<commit_message>
Check StudentID = StudentName upload page
</commit_message>
<xml_diff>
--- a/public/files/Activities1_1.xlsx
+++ b/public/files/Activities1_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
   <si>
     <t>Academic Year</t>
   </si>
@@ -109,9 +109,6 @@
     <t>2590081115</t>
   </si>
   <si>
-    <t>Chulawee Amnajraungkri</t>
-  </si>
-  <si>
     <t>2590081116</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Joonmin Choi</t>
   </si>
   <si>
-    <t>2590081120</t>
-  </si>
-  <si>
     <t>Kuntanun Taengko</t>
   </si>
   <si>
@@ -266,6 +260,21 @@
   </si>
   <si>
     <t>U</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t>asd123</t>
   </si>
 </sst>
 </file>
@@ -658,8 +667,8 @@
   </sheetPr>
   <dimension ref="A1:AN38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -864,10 +873,10 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -878,13 +887,16 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
         <v>83</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
@@ -894,6 +906,9 @@
       <c r="B10" t="s">
         <v>25</v>
       </c>
+      <c r="G10" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -902,6 +917,9 @@
       <c r="B11" t="s">
         <v>27</v>
       </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -916,207 +934,207 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>